<commit_message>
Wrote the implementation to 6 more test cases and modified the xls file so it is up to date with the changes.
</commit_message>
<xml_diff>
--- a/Docs/Lab2/Lab02_BBT_TCs_Form.xls.xlsx
+++ b/Docs/Lab2/Lab02_BBT_TCs_Form.xls.xlsx
@@ -19,19 +19,19 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="G18">
+    <comment authorId="0" ref="G20">
       <text>
         <t xml:space="preserve">Author:
 fill with YES or n/a after debugging</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H18">
+    <comment authorId="0" ref="H20">
       <text>
         <t xml:space="preserve">Author:
 fill with DONE or n/a after re-testing</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J18">
+    <comment authorId="0" ref="J20">
       <text>
         <t xml:space="preserve">Author:
 fill with DONE or n/a after regression testing
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="142">
   <si>
     <t>do not print this form</t>
   </si>
@@ -277,138 +277,6 @@
     <t>12. domeniu: "B...", length = 31</t>
   </si>
   <si>
-    <t>BBT TCs</t>
-  </si>
-  <si>
-    <t>Final        TC No.</t>
-  </si>
-  <si>
-    <t>Req. ID</t>
-  </si>
-  <si>
-    <t>ECP TCs</t>
-  </si>
-  <si>
-    <t>BVA TCs</t>
-  </si>
-  <si>
-    <t>expected</t>
-  </si>
-  <si>
-    <t>actual result</t>
-  </si>
-  <si>
-    <t>Req01</t>
-  </si>
-  <si>
-    <t>TC1_ECP</t>
-  </si>
-  <si>
-    <t>{
-                "1) D-aia.",
-                "2) Da.",
-                "3) Nu."
-}</t>
-  </si>
-  <si>
-    <t>TC3_ECP</t>
-  </si>
-  <si>
-    <t>TC08_BVA</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>TC09_BVA</t>
-  </si>
-  <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Debugging</t>
-  </si>
-  <si>
-    <t>Re-testing</t>
-  </si>
-  <si>
-    <t>Regression Testing</t>
-  </si>
-  <si>
-    <t>#TCs to be run</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#TCs </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color rgb="FF008000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#TCs    </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>failed</t>
-    </r>
-  </si>
-  <si>
-    <t>#Bugs</t>
-  </si>
-  <si>
-    <t>#Bugs Fixed</t>
-  </si>
-  <si>
-    <t>Re-tested</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#TCs </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color rgb="FF008000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#TCs    </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>failed</t>
-    </r>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <rFont val="Calibri"/>
@@ -429,9 +297,6 @@
   </si>
   <si>
     <t>EC Identification</t>
-  </si>
-  <si>
-    <t>not yet</t>
   </si>
   <si>
     <t>EC-based TCs</t>
@@ -458,10 +323,20 @@
     <t>&lt;- see condition</t>
   </si>
   <si>
+    <t>expected</t>
+  </si>
+  <si>
     <t>! condition</t>
   </si>
   <si>
     <t>1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>{
+                "1) D-aia.",
+                "2) Da.",
+                "3) Nu."
+}</t>
   </si>
   <si>
     <t>lista raspunsuri is a string list with a length of 3, containing any symbol. The answers are strings between 3 and 100 characters, starting with "1)", "2)" sau "3)"</t>
@@ -562,12 +437,155 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>BBT TCs</t>
+  </si>
+  <si>
+    <t>Final        TC No.</t>
+  </si>
+  <si>
+    <t>Req. ID</t>
+  </si>
+  <si>
+    <t>ECP TCs</t>
+  </si>
+  <si>
+    <t>BVA TCs</t>
+  </si>
+  <si>
+    <t>actual result</t>
+  </si>
+  <si>
+    <t>Req01</t>
+  </si>
+  <si>
+    <t>TC1_ECP</t>
+  </si>
+  <si>
+    <t>TC2_ECP</t>
+  </si>
+  <si>
+    <t>TC08_BVA</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>TC09_BVA</t>
+  </si>
+  <si>
+    <t>TC4_ECP</t>
+  </si>
+  <si>
+    <t>TC5_ECP</t>
+  </si>
+  <si>
+    <t>TC9_ECP</t>
+  </si>
+  <si>
+    <t>TC10_BVA</t>
+  </si>
+  <si>
+    <t>TC11_BVA</t>
+  </si>
+  <si>
+    <t>TC12_BVA</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Re-testing</t>
+  </si>
+  <si>
+    <t>Regression Testing</t>
+  </si>
+  <si>
+    <t>#TCs to be run</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#TCs </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF008000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#TCs    </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>failed</t>
+    </r>
+  </si>
+  <si>
+    <t>#Bugs</t>
+  </si>
+  <si>
+    <t>#Bugs Fixed</t>
+  </si>
+  <si>
+    <t>Re-tested</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#TCs </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF008000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#TCs    </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>failed</t>
+    </r>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>not yet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -623,7 +641,11 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF0066CC"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF31859B"/>
       <name val="Calibri"/>
@@ -637,16 +659,6 @@
       <i/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF0066CC"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF31859B"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1081,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="133">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1289,6 +1301,48 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -1299,9 +1353,6 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1322,38 +1373,23 @@
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1398,25 +1434,19 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="34" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="35" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="35" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="36" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="36" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="33" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="33" fillId="9" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -1424,38 +1454,8 @@
     <xf borderId="34" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2693,7 +2693,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="B3" s="18" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2709,14 +2709,14 @@
       <c r="M4" s="17"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="120" t="s">
-        <v>99</v>
+      <c r="B5" s="73" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="G5" s="21" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -2728,30 +2728,30 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="B6" s="35" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="I6" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="77" t="s">
+      <c r="M6" s="74" t="s">
         <v>33</v>
       </c>
       <c r="N6" s="4"/>
@@ -2761,12 +2761,12 @@
         <v>1.0</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="123" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="126"/>
+        <v>78</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="76"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="32" t="s">
@@ -2781,8 +2781,8 @@
       <c r="L7" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="77" t="s">
-        <v>75</v>
+      <c r="M7" s="74" t="s">
+        <v>80</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -2791,29 +2791,29 @@
         <v>2.0</v>
       </c>
       <c r="C8" s="31"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="123" t="s">
-        <v>109</v>
+      <c r="D8" s="76"/>
+      <c r="E8" s="75" t="s">
+        <v>81</v>
       </c>
       <c r="G8" s="35">
         <v>1.0</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="I8" s="38" t="s">
         <v>54</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="86">
+        <v>83</v>
+      </c>
+      <c r="K8" s="77">
         <v>1.0</v>
       </c>
       <c r="L8" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="128" t="s">
+      <c r="M8" s="78" t="s">
         <v>49</v>
       </c>
       <c r="N8" s="4"/>
@@ -2823,23 +2823,23 @@
         <v>3.0</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="123" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="126"/>
+        <v>84</v>
+      </c>
+      <c r="D9" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="76"/>
       <c r="G9" s="35">
         <v>2.0</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="I9" s="38" t="s">
         <v>41</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K9" s="30">
         <v>1.0</v>
@@ -2857,21 +2857,21 @@
         <v>4.0</v>
       </c>
       <c r="C10" s="31"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="123" t="s">
-        <v>109</v>
+      <c r="D10" s="76"/>
+      <c r="E10" s="75" t="s">
+        <v>81</v>
       </c>
       <c r="G10" s="35">
         <v>3.0</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="I10" s="38" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="K10" s="30">
         <v>1.0</v>
@@ -2889,23 +2889,23 @@
         <v>5.0</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="123" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="126"/>
+        <v>89</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="76"/>
       <c r="G11" s="35">
         <v>4.0</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="K11" s="30">
         <v>1.0</v>
@@ -2923,21 +2923,21 @@
         <v>6.0</v>
       </c>
       <c r="C12" s="31"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="123" t="s">
-        <v>119</v>
+      <c r="D12" s="76"/>
+      <c r="E12" s="75" t="s">
+        <v>92</v>
       </c>
       <c r="G12" s="35">
         <v>5.0</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="K12" s="30">
         <v>1.0</v>
@@ -2955,23 +2955,23 @@
         <v>7.0</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="126" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="126"/>
+        <v>94</v>
+      </c>
+      <c r="D13" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="76"/>
       <c r="G13" s="35">
         <v>6.0</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>54</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="K13" s="30">
         <v>1.0</v>
@@ -2989,21 +2989,21 @@
         <v>8.0</v>
       </c>
       <c r="C14" s="31"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126" t="s">
-        <v>125</v>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76" t="s">
+        <v>98</v>
       </c>
       <c r="G14" s="35">
         <v>7.0</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="I14" s="38" t="s">
         <v>54</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="K14" s="30">
         <v>1.0</v>
@@ -3018,25 +3018,25 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="B15" s="23"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
       <c r="G15" s="35">
         <v>8.0</v>
       </c>
-      <c r="H15" s="130" t="s">
-        <v>123</v>
+      <c r="H15" s="80" t="s">
+        <v>96</v>
       </c>
       <c r="I15" s="43" t="s">
         <v>54</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="K15" s="42">
         <v>1.0</v>
       </c>
-      <c r="L15" s="131" t="s">
+      <c r="L15" s="81" t="s">
         <v>43</v>
       </c>
       <c r="M15" s="46" t="s">
@@ -3046,24 +3046,24 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="B16" s="23"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
       <c r="G16" s="49">
         <v>9.0</v>
       </c>
-      <c r="H16" s="130" t="s">
-        <v>123</v>
+      <c r="H16" s="80" t="s">
+        <v>96</v>
       </c>
       <c r="I16" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="131" t="s">
-        <v>128</v>
+      <c r="J16" s="81" t="s">
+        <v>101</v>
       </c>
       <c r="K16" s="42">
         <v>1.0</v>
       </c>
-      <c r="L16" s="131" t="s">
+      <c r="L16" s="81" t="s">
         <v>43</v>
       </c>
       <c r="M16" s="46" t="s">
@@ -3073,25 +3073,25 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="B17" s="23"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
       <c r="G17" s="49">
         <v>10.0</v>
       </c>
-      <c r="H17" s="130" t="s">
-        <v>123</v>
+      <c r="H17" s="80" t="s">
+        <v>96</v>
       </c>
       <c r="I17" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="132" t="s">
-        <v>129</v>
+      <c r="J17" s="82" t="s">
+        <v>102</v>
       </c>
       <c r="K17" s="42">
         <v>1.0</v>
       </c>
-      <c r="L17" s="131" t="s">
+      <c r="L17" s="81" t="s">
         <v>43</v>
       </c>
       <c r="M17" s="46" t="s">
@@ -3101,83 +3101,83 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="B18" s="23"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
       <c r="G18" s="49">
         <v>11.0</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="I18" s="38" t="s">
         <v>54</v>
       </c>
       <c r="J18" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="86">
+        <v>83</v>
+      </c>
+      <c r="K18" s="77">
         <v>5.0</v>
       </c>
       <c r="L18" s="30" t="s">
         <v>43</v>
       </c>
       <c r="M18" s="40" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="B19" s="23"/>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
       <c r="G19" s="49">
         <v>12.0</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="I19" s="38" t="s">
         <v>54</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" s="86">
+        <v>83</v>
+      </c>
+      <c r="K19" s="77">
         <v>1.0</v>
       </c>
       <c r="L19" s="30" t="s">
         <v>41</v>
       </c>
       <c r="M19" s="40" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="N19" s="4"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="B20" s="23"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="G20" s="133">
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="G20" s="83">
         <v>13.0</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="I20" s="38" t="s">
         <v>54</v>
       </c>
       <c r="J20" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="K20" s="86">
+        <v>83</v>
+      </c>
+      <c r="K20" s="77">
         <v>1.0</v>
       </c>
       <c r="L20" s="38" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="M20" s="40" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="N20" s="4"/>
     </row>
@@ -3189,10 +3189,10 @@
     <row r="22" ht="14.25" customHeight="1">
       <c r="C22" s="16"/>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="F22" s="68"/>
-      <c r="H22" s="134"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -3204,7 +3204,7 @@
       <c r="C23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
-      <c r="H23" s="135"/>
+      <c r="H23" s="85"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -3216,7 +3216,7 @@
       <c r="C24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
-      <c r="H24" s="136"/>
+      <c r="H24" s="86"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -8106,39 +8106,39 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="C19:C20"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:N22"/>
     <mergeCell ref="H23:N23"/>
     <mergeCell ref="H24:N24"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G5:N5"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M9:N9"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -13677,25 +13677,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="D1:G1"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:P5"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O7:P7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="O8:P8"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O11:P11"/>
     <mergeCell ref="O12:P12"/>
-    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="O14:P14"/>
@@ -13704,20 +13710,14 @@
     <mergeCell ref="C17:C22"/>
     <mergeCell ref="D17:D22"/>
     <mergeCell ref="D25:D28"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C28"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="O23:P23"/>
     <mergeCell ref="I26:M26"/>
     <mergeCell ref="I27:M27"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -13737,7 +13737,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="8.0"/>
+    <col customWidth="1" min="1" max="3" width="8.0"/>
+    <col customWidth="1" min="4" max="4" width="13.0"/>
+    <col customWidth="1" min="5" max="5" width="20.0"/>
     <col customWidth="1" min="6" max="6" width="12.14"/>
     <col customWidth="1" min="7" max="7" width="17.57"/>
     <col customWidth="1" min="8" max="8" width="26.86"/>
@@ -13752,7 +13754,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="16"/>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="87" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3"/>
@@ -13774,8 +13776,8 @@
       <c r="K2" s="17"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="74" t="s">
-        <v>70</v>
+      <c r="B3" s="88" t="s">
+        <v>109</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -13789,72 +13791,72 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="B4" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="76" t="s">
-        <v>73</v>
+        <v>110</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>112</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="74" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="74" t="s">
         <v>33</v>
       </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5">
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="81" t="s">
+      <c r="B5" s="91"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="81" t="s">
+      <c r="H5" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="81" t="s">
+      <c r="I5" s="94" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" ht="66.75">
-      <c r="B6" s="82">
+      <c r="B6" s="95">
         <v>1.0</v>
       </c>
-      <c r="C6" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="85" t="s">
+      <c r="C6" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="98" t="s">
         <v>63</v>
       </c>
       <c r="F6" s="38" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="86">
+        <v>83</v>
+      </c>
+      <c r="H6" s="77">
         <v>1.0</v>
       </c>
       <c r="I6" s="30" t="s">
@@ -13863,7 +13865,7 @@
       <c r="J6" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="99" t="s">
         <v>49</v>
       </c>
     </row>
@@ -13872,18 +13874,18 @@
         <f t="shared" ref="B7:B13" si="1">B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="90" t="s">
+      <c r="C7" s="100"/>
+      <c r="D7" s="101" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="102" t="s">
         <v>63</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H7" s="30">
         <v>1.0</v>
@@ -13901,10 +13903,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="103"/>
       <c r="E8" s="32" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>54</v>
@@ -13928,12 +13930,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C9" s="88"/>
-      <c r="D9" s="89" t="s">
-        <v>82</v>
+      <c r="C9" s="100"/>
+      <c r="D9" s="103" t="s">
+        <v>119</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="F9" s="47" t="s">
         <v>54</v>
@@ -13957,215 +13959,301 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="90"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="B11" s="35">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="91"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="90"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="101" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="102"/>
+      <c r="F11" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="B12" s="35">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="90"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="95">
+      <c r="C12" s="100"/>
+      <c r="D12" s="101" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="102"/>
+      <c r="F12" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="I12" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" ht="27.0">
+      <c r="B13" s="104">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="B14" s="49">
+        <v>9.0</v>
+      </c>
+      <c r="C14" s="100"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="I14" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="B15" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="17"/>
+      <c r="B15" s="49">
+        <v>10.0</v>
+      </c>
+      <c r="C15" s="92"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="I15" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="4"/>
     </row>
     <row r="16">
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="17"/>
-    </row>
-    <row r="17">
-      <c r="C17" s="100" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="103" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" s="104" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="102"/>
-      <c r="J17" s="104" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="101"/>
-      <c r="L17" s="101"/>
-      <c r="M17" s="102"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="105" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="106" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="107" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="108" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="61"/>
-      <c r="J18" s="106" t="s">
-        <v>94</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="L18" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="M18" s="75" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="109"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="114"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="111"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="106"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="B17" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="62"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="107"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19">
+      <c r="C19" s="108" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="111" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="110"/>
+      <c r="J19" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="110"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="B20" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="116">
-        <f>SUM(D20:E20)</f>
+      <c r="B20" s="113" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="114" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="115" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="116" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" s="61"/>
+      <c r="J20" s="114" t="s">
+        <v>137</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="M20" s="89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="B21" s="117"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="120"/>
+      <c r="H21" s="121"/>
+      <c r="I21" s="122"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="119"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="B22" s="123" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="124">
+        <f>SUM(D22:E22)</f>
+        <v>10</v>
+      </c>
+      <c r="D22" s="125">
+        <v>10.0</v>
+      </c>
+      <c r="E22" s="125">
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="126">
+        <v>0.0</v>
+      </c>
+      <c r="G22" s="127" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="129" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" s="47">
+        <f>SUM(L22:M22)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="117"/>
-      <c r="E20" s="117"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="119" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" s="121" t="s">
-        <v>100</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="122" t="s">
-        <v>100</v>
-      </c>
-      <c r="K20" s="47">
-        <f>SUM(L20:M20)</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="124"/>
-      <c r="M20" s="125"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="L22" s="130"/>
+      <c r="M22" s="131"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="D23" s="17"/>
@@ -14174,7 +14262,7 @@
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="J23" s="132"/>
       <c r="K23" s="17"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -23947,35 +24035,61 @@
       <c r="J1000" s="17"/>
       <c r="K1000" s="17"/>
     </row>
+    <row r="1001" ht="14.25" customHeight="1">
+      <c r="D1001" s="17"/>
+      <c r="E1001" s="17"/>
+      <c r="F1001" s="17"/>
+      <c r="G1001" s="17"/>
+      <c r="H1001" s="17"/>
+      <c r="I1001" s="17"/>
+      <c r="J1001" s="17"/>
+      <c r="K1001" s="17"/>
+    </row>
+    <row r="1002" ht="14.25" customHeight="1">
+      <c r="D1002" s="17"/>
+      <c r="E1002" s="17"/>
+      <c r="F1002" s="17"/>
+      <c r="G1002" s="17"/>
+      <c r="H1002" s="17"/>
+      <c r="I1002" s="17"/>
+      <c r="J1002" s="17"/>
+      <c r="K1002" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="33">
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C6:C15"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="F4:I4"/>
+    <mergeCell ref="H20:I21"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="J19:M19"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="J9:K9"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>